<commit_message>
jacobipar and jacobiseq allows user to test a equation with the calculated answer
</commit_message>
<xml_diff>
--- a/analysis_windows.xlsx
+++ b/analysis_windows.xlsx
@@ -8,13 +8,19 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Git\jacobipar-concurrent-programming\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{688FC6F8-1D61-411C-A9D7-3EB8E03A9444}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{ADC0479F-C49D-4344-B129-266602944A1C}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15990" xr2:uid="{5F68885C-97C5-46B4-BB9B-B07ABA363B16}"/>
   </bookViews>
   <sheets>
     <sheet name="Planilha1" sheetId="1" r:id="rId1"/>
   </sheets>
+  <definedNames>
+    <definedName name="_xlchart.v1.0" hidden="1">Planilha1!$M$6:$M$8</definedName>
+    <definedName name="_xlchart.v1.1" hidden="1">Planilha1!$N$6:$N$8</definedName>
+    <definedName name="_xlchart.v1.2" hidden="1">Planilha1!$P$6:$P$8</definedName>
+    <definedName name="_xlchart.v1.3" hidden="1">Planilha1!$R$6:$R$8</definedName>
+  </definedNames>
   <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
@@ -55,7 +61,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1089" uniqueCount="9">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1365" uniqueCount="23">
   <si>
     <t>N</t>
   </si>
@@ -82,6 +88,48 @@
   </si>
   <si>
     <t>Speedup</t>
+  </si>
+  <si>
+    <t>B max error:    0.00088</t>
+  </si>
+  <si>
+    <t>B max error:    0.00099</t>
+  </si>
+  <si>
+    <t>B max error:    0.00090</t>
+  </si>
+  <si>
+    <t>B max error:    0.00116</t>
+  </si>
+  <si>
+    <t>B max error:    0.00087</t>
+  </si>
+  <si>
+    <t>B max error:    0.00085</t>
+  </si>
+  <si>
+    <t>B max error:    0.00083</t>
+  </si>
+  <si>
+    <t>B max error:    0.00086</t>
+  </si>
+  <si>
+    <t>B max error:    0.00084</t>
+  </si>
+  <si>
+    <t>B max error:    0.00089</t>
+  </si>
+  <si>
+    <t>B max error:    0.00091</t>
+  </si>
+  <si>
+    <t>B max error:    0.00082</t>
+  </si>
+  <si>
+    <t>B max error:    0.00081</t>
+  </si>
+  <si>
+    <t>Eficiência</t>
   </si>
 </sst>
 </file>
@@ -120,11 +168,12 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center"/>
+      <alignment vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -167,6 +216,9 @@
         <c:ser>
           <c:idx val="0"/>
           <c:order val="0"/>
+          <c:tx>
+            <c:v>12 threads</c:v>
+          </c:tx>
           <c:spPr>
             <a:solidFill>
               <a:schemeClr val="accent1"/>
@@ -208,6 +260,7 @@
                 <a:endParaRPr lang="pt-BR"/>
               </a:p>
             </c:txPr>
+            <c:dLblPos val="outEnd"/>
             <c:showLegendKey val="0"/>
             <c:showVal val="1"/>
             <c:showCatName val="0"/>
@@ -235,9 +288,63 @@
               </c:ext>
             </c:extLst>
           </c:dLbls>
+          <c:errBars>
+            <c:errBarType val="both"/>
+            <c:errValType val="cust"/>
+            <c:noEndCap val="0"/>
+            <c:plus>
+              <c:numRef>
+                <c:f>Planilha1!$O$6:$O$8</c:f>
+                <c:numCache>
+                  <c:formatCode>General</c:formatCode>
+                  <c:ptCount val="3"/>
+                  <c:pt idx="0">
+                    <c:v>6.3391656090751713E-3</c:v>
+                  </c:pt>
+                  <c:pt idx="1">
+                    <c:v>7.5131583248602947E-3</c:v>
+                  </c:pt>
+                  <c:pt idx="2">
+                    <c:v>7.1096512154603907E-3</c:v>
+                  </c:pt>
+                </c:numCache>
+              </c:numRef>
+            </c:plus>
+            <c:minus>
+              <c:numRef>
+                <c:f>Planilha1!$O$6:$O$8</c:f>
+                <c:numCache>
+                  <c:formatCode>General</c:formatCode>
+                  <c:ptCount val="3"/>
+                  <c:pt idx="0">
+                    <c:v>6.3391656090751713E-3</c:v>
+                  </c:pt>
+                  <c:pt idx="1">
+                    <c:v>7.5131583248602947E-3</c:v>
+                  </c:pt>
+                  <c:pt idx="2">
+                    <c:v>7.1096512154603907E-3</c:v>
+                  </c:pt>
+                </c:numCache>
+              </c:numRef>
+            </c:minus>
+            <c:spPr>
+              <a:noFill/>
+              <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:round/>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+          </c:errBars>
           <c:val>
             <c:numRef>
-              <c:f>(Planilha1!$N$6,Planilha1!$P$6,Planilha1!$R$6)</c:f>
+              <c:f>Planilha1!$N$6:$N$8</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="3"/>
@@ -245,23 +352,26 @@
                   <c:v>1.2433330209999999E-2</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>2.1766646689999992E-2</c:v>
+                  <c:v>3.636666932333333E-2</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>1.9217000166566665</c:v>
+                  <c:v>0.18626665272999998</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
           </c:val>
           <c:extLst>
             <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
-              <c16:uniqueId val="{00000000-383C-48EF-BB5B-8D6F3F88BF97}"/>
+              <c16:uniqueId val="{00000000-5C32-41F2-BE28-F05BB45219FE}"/>
             </c:ext>
           </c:extLst>
         </c:ser>
         <c:ser>
           <c:idx val="1"/>
           <c:order val="1"/>
+          <c:tx>
+            <c:v>50 threads</c:v>
+          </c:tx>
           <c:spPr>
             <a:solidFill>
               <a:schemeClr val="accent2"/>
@@ -331,33 +441,81 @@
               </c:ext>
             </c:extLst>
           </c:dLbls>
+          <c:errBars>
+            <c:errBarType val="both"/>
+            <c:errValType val="cust"/>
+            <c:noEndCap val="0"/>
+            <c:plus>
+              <c:numRef>
+                <c:f>Planilha1!$Q$6:$Q$8</c:f>
+                <c:numCache>
+                  <c:formatCode>General</c:formatCode>
+                  <c:ptCount val="3"/>
+                  <c:pt idx="0">
+                    <c:v>7.8901561331726332E-3</c:v>
+                  </c:pt>
+                  <c:pt idx="1">
+                    <c:v>5.0398616965780885E-4</c:v>
+                  </c:pt>
+                  <c:pt idx="2">
+                    <c:v>4.9826980767722227E-4</c:v>
+                  </c:pt>
+                </c:numCache>
+              </c:numRef>
+            </c:plus>
+            <c:minus>
+              <c:numLit>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>1</c:v>
+                </c:pt>
+              </c:numLit>
+            </c:minus>
+            <c:spPr>
+              <a:noFill/>
+              <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:round/>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+          </c:errBars>
           <c:val>
             <c:numRef>
-              <c:f>(Planilha1!$N$7,Planilha1!$P$7,Planilha1!$R$7)</c:f>
+              <c:f>Planilha1!$P$6:$P$8</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="3"/>
                 <c:pt idx="0">
-                  <c:v>3.636666932333333E-2</c:v>
+                  <c:v>2.1766646689999992E-2</c:v>
                 </c:pt>
                 <c:pt idx="1">
                   <c:v>1.5566674856666664E-2</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>3.066666124E-2</c:v>
+                  <c:v>6.2400007240000013E-2</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
           </c:val>
           <c:extLst>
             <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
-              <c16:uniqueId val="{00000001-383C-48EF-BB5B-8D6F3F88BF97}"/>
+              <c16:uniqueId val="{00000001-5C32-41F2-BE28-F05BB45219FE}"/>
             </c:ext>
           </c:extLst>
         </c:ser>
         <c:ser>
           <c:idx val="2"/>
           <c:order val="2"/>
+          <c:tx>
+            <c:v>100 threads</c:v>
+          </c:tx>
           <c:spPr>
             <a:solidFill>
               <a:schemeClr val="accent3"/>
@@ -427,17 +585,71 @@
               </c:ext>
             </c:extLst>
           </c:dLbls>
+          <c:errBars>
+            <c:errBarType val="both"/>
+            <c:errValType val="cust"/>
+            <c:noEndCap val="0"/>
+            <c:plus>
+              <c:numRef>
+                <c:f>Planilha1!$S$6:$S$8</c:f>
+                <c:numCache>
+                  <c:formatCode>General</c:formatCode>
+                  <c:ptCount val="3"/>
+                  <c:pt idx="0">
+                    <c:v>6.9947858318567133E-2</c:v>
+                  </c:pt>
+                  <c:pt idx="1">
+                    <c:v>2.795718900439597E-3</c:v>
+                  </c:pt>
+                  <c:pt idx="2">
+                    <c:v>4.0683287497980707E-4</c:v>
+                  </c:pt>
+                </c:numCache>
+              </c:numRef>
+            </c:plus>
+            <c:minus>
+              <c:numRef>
+                <c:f>Planilha1!$S$6:$S$8</c:f>
+                <c:numCache>
+                  <c:formatCode>General</c:formatCode>
+                  <c:ptCount val="3"/>
+                  <c:pt idx="0">
+                    <c:v>6.9947858318567133E-2</c:v>
+                  </c:pt>
+                  <c:pt idx="1">
+                    <c:v>2.795718900439597E-3</c:v>
+                  </c:pt>
+                  <c:pt idx="2">
+                    <c:v>4.0683287497980707E-4</c:v>
+                  </c:pt>
+                </c:numCache>
+              </c:numRef>
+            </c:minus>
+            <c:spPr>
+              <a:noFill/>
+              <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:round/>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+          </c:errBars>
           <c:val>
             <c:numRef>
-              <c:f>(Planilha1!$N$8,Planilha1!$P$8,Planilha1!$R$8)</c:f>
+              <c:f>Planilha1!$R$6:$R$8</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="3"/>
                 <c:pt idx="0">
-                  <c:v>0.18626665272999998</c:v>
+                  <c:v>1.9217000166566665</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>6.2400007240000013E-2</c:v>
+                  <c:v>3.066666124E-2</c:v>
                 </c:pt>
                 <c:pt idx="2">
                   <c:v>4.6799993500000005E-2</c:v>
@@ -447,59 +659,353 @@
           </c:val>
           <c:extLst>
             <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
-              <c16:uniqueId val="{00000002-383C-48EF-BB5B-8D6F3F88BF97}"/>
+              <c16:uniqueId val="{00000002-5C32-41F2-BE28-F05BB45219FE}"/>
             </c:ext>
           </c:extLst>
         </c:ser>
         <c:dLbls>
+          <c:dLblPos val="outEnd"/>
           <c:showLegendKey val="0"/>
-          <c:showVal val="0"/>
+          <c:showVal val="1"/>
           <c:showCatName val="0"/>
           <c:showSerName val="0"/>
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:gapWidth val="300"/>
-        <c:axId val="418291120"/>
-        <c:axId val="418293088"/>
+        <c:gapWidth val="219"/>
+        <c:overlap val="-27"/>
+        <c:axId val="410963952"/>
+        <c:axId val="410961328"/>
+        <c:extLst>
+          <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{02D57815-91ED-43cb-92C2-25804820EDAC}">
+            <c15:filteredBarSeries>
+              <c15:ser>
+                <c:idx val="3"/>
+                <c:order val="3"/>
+                <c:tx>
+                  <c:v>12 stdev</c:v>
+                </c:tx>
+                <c:spPr>
+                  <a:solidFill>
+                    <a:schemeClr val="accent4"/>
+                  </a:solidFill>
+                  <a:ln>
+                    <a:noFill/>
+                  </a:ln>
+                  <a:effectLst/>
+                </c:spPr>
+                <c:invertIfNegative val="0"/>
+                <c:dLbls>
+                  <c:spPr>
+                    <a:noFill/>
+                    <a:ln>
+                      <a:noFill/>
+                    </a:ln>
+                    <a:effectLst/>
+                  </c:spPr>
+                  <c:txPr>
+                    <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" lIns="38100" tIns="19050" rIns="38100" bIns="19050" anchor="ctr" anchorCtr="1">
+                      <a:spAutoFit/>
+                    </a:bodyPr>
+                    <a:lstStyle/>
+                    <a:p>
+                      <a:pPr>
+                        <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                          <a:solidFill>
+                            <a:schemeClr val="tx1">
+                              <a:lumMod val="75000"/>
+                              <a:lumOff val="25000"/>
+                            </a:schemeClr>
+                          </a:solidFill>
+                          <a:latin typeface="+mn-lt"/>
+                          <a:ea typeface="+mn-ea"/>
+                          <a:cs typeface="+mn-cs"/>
+                        </a:defRPr>
+                      </a:pPr>
+                      <a:endParaRPr lang="pt-BR"/>
+                    </a:p>
+                  </c:txPr>
+                  <c:dLblPos val="outEnd"/>
+                  <c:showLegendKey val="0"/>
+                  <c:showVal val="1"/>
+                  <c:showCatName val="0"/>
+                  <c:showSerName val="0"/>
+                  <c:showPercent val="0"/>
+                  <c:showBubbleSize val="0"/>
+                  <c:showLeaderLines val="0"/>
+                  <c:extLst>
+                    <c:ext uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
+                      <c15:showLeaderLines val="1"/>
+                      <c15:leaderLines>
+                        <c:spPr>
+                          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+                            <a:solidFill>
+                              <a:schemeClr val="tx1">
+                                <a:lumMod val="35000"/>
+                                <a:lumOff val="65000"/>
+                              </a:schemeClr>
+                            </a:solidFill>
+                            <a:round/>
+                          </a:ln>
+                          <a:effectLst/>
+                        </c:spPr>
+                      </c15:leaderLines>
+                    </c:ext>
+                  </c:extLst>
+                </c:dLbls>
+                <c:val>
+                  <c:numRef>
+                    <c:extLst>
+                      <c:ext uri="{02D57815-91ED-43cb-92C2-25804820EDAC}">
+                        <c15:formulaRef>
+                          <c15:sqref>Planilha1!$O$6:$O$8</c15:sqref>
+                        </c15:formulaRef>
+                      </c:ext>
+                    </c:extLst>
+                    <c:numCache>
+                      <c:formatCode>General</c:formatCode>
+                      <c:ptCount val="3"/>
+                      <c:pt idx="0">
+                        <c:v>6.3391656090751713E-3</c:v>
+                      </c:pt>
+                      <c:pt idx="1">
+                        <c:v>7.5131583248602947E-3</c:v>
+                      </c:pt>
+                      <c:pt idx="2">
+                        <c:v>7.1096512154603907E-3</c:v>
+                      </c:pt>
+                    </c:numCache>
+                  </c:numRef>
+                </c:val>
+                <c:extLst>
+                  <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+                    <c16:uniqueId val="{00000004-5C32-41F2-BE28-F05BB45219FE}"/>
+                  </c:ext>
+                </c:extLst>
+              </c15:ser>
+            </c15:filteredBarSeries>
+            <c15:filteredBarSeries>
+              <c15:ser>
+                <c:idx val="4"/>
+                <c:order val="4"/>
+                <c:tx>
+                  <c:v>50 stdev</c:v>
+                </c:tx>
+                <c:spPr>
+                  <a:solidFill>
+                    <a:schemeClr val="accent5"/>
+                  </a:solidFill>
+                  <a:ln>
+                    <a:noFill/>
+                  </a:ln>
+                  <a:effectLst/>
+                </c:spPr>
+                <c:invertIfNegative val="0"/>
+                <c:dLbls>
+                  <c:spPr>
+                    <a:noFill/>
+                    <a:ln>
+                      <a:noFill/>
+                    </a:ln>
+                    <a:effectLst/>
+                  </c:spPr>
+                  <c:txPr>
+                    <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" lIns="38100" tIns="19050" rIns="38100" bIns="19050" anchor="ctr" anchorCtr="1">
+                      <a:spAutoFit/>
+                    </a:bodyPr>
+                    <a:lstStyle/>
+                    <a:p>
+                      <a:pPr>
+                        <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                          <a:solidFill>
+                            <a:schemeClr val="tx1">
+                              <a:lumMod val="75000"/>
+                              <a:lumOff val="25000"/>
+                            </a:schemeClr>
+                          </a:solidFill>
+                          <a:latin typeface="+mn-lt"/>
+                          <a:ea typeface="+mn-ea"/>
+                          <a:cs typeface="+mn-cs"/>
+                        </a:defRPr>
+                      </a:pPr>
+                      <a:endParaRPr lang="pt-BR"/>
+                    </a:p>
+                  </c:txPr>
+                  <c:dLblPos val="outEnd"/>
+                  <c:showLegendKey val="0"/>
+                  <c:showVal val="1"/>
+                  <c:showCatName val="0"/>
+                  <c:showSerName val="0"/>
+                  <c:showPercent val="0"/>
+                  <c:showBubbleSize val="0"/>
+                  <c:showLeaderLines val="0"/>
+                  <c:extLst>
+                    <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
+                      <c15:showLeaderLines val="1"/>
+                      <c15:leaderLines>
+                        <c:spPr>
+                          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+                            <a:solidFill>
+                              <a:schemeClr val="tx1">
+                                <a:lumMod val="35000"/>
+                                <a:lumOff val="65000"/>
+                              </a:schemeClr>
+                            </a:solidFill>
+                            <a:round/>
+                          </a:ln>
+                          <a:effectLst/>
+                        </c:spPr>
+                      </c15:leaderLines>
+                    </c:ext>
+                  </c:extLst>
+                </c:dLbls>
+                <c:val>
+                  <c:numRef>
+                    <c:extLst>
+                      <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{02D57815-91ED-43cb-92C2-25804820EDAC}">
+                        <c15:formulaRef>
+                          <c15:sqref>Planilha1!$Q$6:$Q$8</c15:sqref>
+                        </c15:formulaRef>
+                      </c:ext>
+                    </c:extLst>
+                    <c:numCache>
+                      <c:formatCode>General</c:formatCode>
+                      <c:ptCount val="3"/>
+                      <c:pt idx="0">
+                        <c:v>7.8901561331726332E-3</c:v>
+                      </c:pt>
+                      <c:pt idx="1">
+                        <c:v>5.0398616965780885E-4</c:v>
+                      </c:pt>
+                      <c:pt idx="2">
+                        <c:v>4.9826980767722227E-4</c:v>
+                      </c:pt>
+                    </c:numCache>
+                  </c:numRef>
+                </c:val>
+                <c:extLst>
+                  <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+                    <c16:uniqueId val="{00000005-5C32-41F2-BE28-F05BB45219FE}"/>
+                  </c:ext>
+                </c:extLst>
+              </c15:ser>
+            </c15:filteredBarSeries>
+            <c15:filteredBarSeries>
+              <c15:ser>
+                <c:idx val="5"/>
+                <c:order val="5"/>
+                <c:tx>
+                  <c:v>100 stdev</c:v>
+                </c:tx>
+                <c:spPr>
+                  <a:solidFill>
+                    <a:schemeClr val="accent6"/>
+                  </a:solidFill>
+                  <a:ln>
+                    <a:noFill/>
+                  </a:ln>
+                  <a:effectLst/>
+                </c:spPr>
+                <c:invertIfNegative val="0"/>
+                <c:dLbls>
+                  <c:spPr>
+                    <a:noFill/>
+                    <a:ln>
+                      <a:noFill/>
+                    </a:ln>
+                    <a:effectLst/>
+                  </c:spPr>
+                  <c:txPr>
+                    <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" lIns="38100" tIns="19050" rIns="38100" bIns="19050" anchor="ctr" anchorCtr="1">
+                      <a:spAutoFit/>
+                    </a:bodyPr>
+                    <a:lstStyle/>
+                    <a:p>
+                      <a:pPr>
+                        <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                          <a:solidFill>
+                            <a:schemeClr val="tx1">
+                              <a:lumMod val="75000"/>
+                              <a:lumOff val="25000"/>
+                            </a:schemeClr>
+                          </a:solidFill>
+                          <a:latin typeface="+mn-lt"/>
+                          <a:ea typeface="+mn-ea"/>
+                          <a:cs typeface="+mn-cs"/>
+                        </a:defRPr>
+                      </a:pPr>
+                      <a:endParaRPr lang="pt-BR"/>
+                    </a:p>
+                  </c:txPr>
+                  <c:dLblPos val="outEnd"/>
+                  <c:showLegendKey val="0"/>
+                  <c:showVal val="1"/>
+                  <c:showCatName val="0"/>
+                  <c:showSerName val="0"/>
+                  <c:showPercent val="0"/>
+                  <c:showBubbleSize val="0"/>
+                  <c:showLeaderLines val="0"/>
+                  <c:extLst>
+                    <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
+                      <c15:showLeaderLines val="1"/>
+                      <c15:leaderLines>
+                        <c:spPr>
+                          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+                            <a:solidFill>
+                              <a:schemeClr val="tx1">
+                                <a:lumMod val="35000"/>
+                                <a:lumOff val="65000"/>
+                              </a:schemeClr>
+                            </a:solidFill>
+                            <a:round/>
+                          </a:ln>
+                          <a:effectLst/>
+                        </c:spPr>
+                      </c15:leaderLines>
+                    </c:ext>
+                  </c:extLst>
+                </c:dLbls>
+                <c:val>
+                  <c:numRef>
+                    <c:extLst>
+                      <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{02D57815-91ED-43cb-92C2-25804820EDAC}">
+                        <c15:formulaRef>
+                          <c15:sqref>Planilha1!$S$6:$S$8</c15:sqref>
+                        </c15:formulaRef>
+                      </c:ext>
+                    </c:extLst>
+                    <c:numCache>
+                      <c:formatCode>General</c:formatCode>
+                      <c:ptCount val="3"/>
+                      <c:pt idx="0">
+                        <c:v>6.9947858318567133E-2</c:v>
+                      </c:pt>
+                      <c:pt idx="1">
+                        <c:v>2.795718900439597E-3</c:v>
+                      </c:pt>
+                      <c:pt idx="2">
+                        <c:v>4.0683287497980707E-4</c:v>
+                      </c:pt>
+                    </c:numCache>
+                  </c:numRef>
+                </c:val>
+                <c:extLst>
+                  <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+                    <c16:uniqueId val="{00000006-5C32-41F2-BE28-F05BB45219FE}"/>
+                  </c:ext>
+                </c:extLst>
+              </c15:ser>
+            </c15:filteredBarSeries>
+          </c:ext>
+        </c:extLst>
       </c:barChart>
       <c:catAx>
-        <c:axId val="418291120"/>
+        <c:axId val="410963952"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
         <c:delete val="0"/>
         <c:axPos val="b"/>
-        <c:title>
-          <c:overlay val="0"/>
-          <c:spPr>
-            <a:noFill/>
-            <a:ln>
-              <a:noFill/>
-            </a:ln>
-            <a:effectLst/>
-          </c:spPr>
-          <c:txPr>
-            <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
-            <a:lstStyle/>
-            <a:p>
-              <a:pPr>
-                <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
-                  <a:solidFill>
-                    <a:schemeClr val="tx1">
-                      <a:lumMod val="65000"/>
-                      <a:lumOff val="35000"/>
-                    </a:schemeClr>
-                  </a:solidFill>
-                  <a:latin typeface="+mn-lt"/>
-                  <a:ea typeface="+mn-ea"/>
-                  <a:cs typeface="+mn-cs"/>
-                </a:defRPr>
-              </a:pPr>
-              <a:endParaRPr lang="pt-BR"/>
-            </a:p>
-          </c:txPr>
-        </c:title>
         <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
@@ -536,92 +1042,48 @@
             <a:endParaRPr lang="pt-BR"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="418293088"/>
-        <c:crossesAt val="1.0000000000000002E-3"/>
+        <c:crossAx val="410961328"/>
+        <c:crossesAt val="1.0000000000000003E-4"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
         <c:lblOffset val="100"/>
+        <c:tickMarkSkip val="1"/>
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="418293088"/>
+        <c:axId val="410961328"/>
         <c:scaling>
           <c:logBase val="10"/>
           <c:orientation val="minMax"/>
+          <c:max val="10"/>
+          <c:min val="1.0000000000000003E-4"/>
         </c:scaling>
         <c:delete val="0"/>
         <c:axPos val="l"/>
         <c:majorGridlines>
           <c:spPr>
             <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-              <a:solidFill>
-                <a:schemeClr val="tx1">
-                  <a:lumMod val="15000"/>
-                  <a:lumOff val="85000"/>
-                </a:schemeClr>
-              </a:solidFill>
+              <a:noFill/>
               <a:round/>
             </a:ln>
             <a:effectLst/>
           </c:spPr>
         </c:majorGridlines>
-        <c:minorGridlines>
-          <c:spPr>
-            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-              <a:solidFill>
-                <a:schemeClr val="tx1">
-                  <a:lumMod val="5000"/>
-                  <a:lumOff val="95000"/>
-                </a:schemeClr>
-              </a:solidFill>
-              <a:round/>
-            </a:ln>
-            <a:effectLst/>
-          </c:spPr>
-        </c:minorGridlines>
-        <c:title>
-          <c:overlay val="0"/>
-          <c:spPr>
-            <a:noFill/>
-            <a:ln>
-              <a:noFill/>
-            </a:ln>
-            <a:effectLst/>
-          </c:spPr>
-          <c:txPr>
-            <a:bodyPr rot="-5400000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
-            <a:lstStyle/>
-            <a:p>
-              <a:pPr>
-                <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
-                  <a:solidFill>
-                    <a:schemeClr val="tx1">
-                      <a:lumMod val="65000"/>
-                      <a:lumOff val="35000"/>
-                    </a:schemeClr>
-                  </a:solidFill>
-                  <a:latin typeface="+mn-lt"/>
-                  <a:ea typeface="+mn-ea"/>
-                  <a:cs typeface="+mn-cs"/>
-                </a:defRPr>
-              </a:pPr>
-              <a:endParaRPr lang="pt-BR"/>
-            </a:p>
-          </c:txPr>
-        </c:title>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:majorTickMark val="out"/>
-        <c:minorTickMark val="none"/>
+        <c:minorTickMark val="in"/>
         <c:tickLblPos val="nextTo"/>
         <c:spPr>
           <a:noFill/>
           <a:ln>
-            <a:noFill/>
+            <a:solidFill>
+              <a:schemeClr val="accent1"/>
+            </a:solidFill>
           </a:ln>
           <a:effectLst/>
         </c:spPr>
         <c:txPr>
-          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="t" anchorCtr="0"/>
           <a:lstStyle/>
           <a:p>
             <a:pPr>
@@ -640,12 +1102,10 @@
             <a:endParaRPr lang="pt-BR"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="418291120"/>
+        <c:crossAx val="410963952"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
-        <c:dispUnits>
-          <c:builtInUnit val="thousands"/>
-        </c:dispUnits>
+        <c:minorUnit val="10"/>
       </c:valAx>
       <c:spPr>
         <a:noFill/>
@@ -656,7 +1116,7 @@
       </c:spPr>
     </c:plotArea>
     <c:legend>
-      <c:legendPos val="r"/>
+      <c:legendPos val="b"/>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -1278,22 +1738,22 @@
   <xdr:twoCellAnchor>
     <xdr:from>
       <xdr:col>11</xdr:col>
-      <xdr:colOff>76200</xdr:colOff>
+      <xdr:colOff>271462</xdr:colOff>
       <xdr:row>20</xdr:row>
       <xdr:rowOff>109537</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>18</xdr:col>
-      <xdr:colOff>381000</xdr:colOff>
+      <xdr:colOff>576262</xdr:colOff>
       <xdr:row>34</xdr:row>
       <xdr:rowOff>185737</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
-        <xdr:cNvPr id="2" name="Gráfico 1">
+        <xdr:cNvPr id="4" name="Gráfico 3">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{5B3630C2-9B85-4D5F-A63B-FAF008233435}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{5A2CF4B9-9FCA-4B5A-BB83-E469D05DFB6B}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -1611,10 +2071,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A1C2F0EE-48DD-4DBB-B1D3-7B040A1D4743}">
-  <dimension ref="C3:S274"/>
+  <dimension ref="C3:Z274"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="D2" workbookViewId="0">
-      <selection activeCell="M11" sqref="M11:O20"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="P16" sqref="P16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1622,7 +2082,7 @@
     <col min="8" max="8" width="19.85546875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="3" spans="3:19" x14ac:dyDescent="0.25">
+    <row r="3" spans="3:26" x14ac:dyDescent="0.25">
       <c r="N3" s="2" t="s">
         <v>7</v>
       </c>
@@ -1632,7 +2092,7 @@
       <c r="R3" s="2"/>
       <c r="S3" s="2"/>
     </row>
-    <row r="4" spans="3:19" x14ac:dyDescent="0.25">
+    <row r="4" spans="3:26" x14ac:dyDescent="0.25">
       <c r="N4" s="2">
         <v>12</v>
       </c>
@@ -1646,7 +2106,7 @@
       </c>
       <c r="S4" s="2"/>
     </row>
-    <row r="5" spans="3:19" x14ac:dyDescent="0.25">
+    <row r="5" spans="3:26" x14ac:dyDescent="0.25">
       <c r="C5" t="s">
         <v>0</v>
       </c>
@@ -1689,8 +2149,23 @@
       <c r="S5" t="s">
         <v>6</v>
       </c>
-    </row>
-    <row r="6" spans="3:19" x14ac:dyDescent="0.25">
+      <c r="V5" t="s">
+        <v>0</v>
+      </c>
+      <c r="W5">
+        <v>100</v>
+      </c>
+      <c r="X5" t="s">
+        <v>2</v>
+      </c>
+      <c r="Y5">
+        <v>8.0000000000000002E-3</v>
+      </c>
+      <c r="Z5" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="6" spans="3:26" x14ac:dyDescent="0.25">
       <c r="C6" t="s">
         <v>0</v>
       </c>
@@ -1715,7 +2190,7 @@
       <c r="J6">
         <v>1.4999999999999999E-4</v>
       </c>
-      <c r="L6" s="2" t="s">
+      <c r="L6" s="3" t="s">
         <v>4</v>
       </c>
       <c r="M6">
@@ -1745,8 +2220,23 @@
         <f t="array" ref="S6">_xlfn.STDEV.S((H65:H94)*0.00001)</f>
         <v>6.9947858318567133E-2</v>
       </c>
-    </row>
-    <row r="7" spans="3:19" x14ac:dyDescent="0.25">
+      <c r="V6" t="s">
+        <v>0</v>
+      </c>
+      <c r="W6">
+        <v>100</v>
+      </c>
+      <c r="X6" t="s">
+        <v>2</v>
+      </c>
+      <c r="Y6">
+        <v>8.0000000000000002E-3</v>
+      </c>
+      <c r="Z6" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="7" spans="3:26" x14ac:dyDescent="0.25">
       <c r="C7" t="s">
         <v>0</v>
       </c>
@@ -1771,7 +2261,7 @@
       <c r="J7">
         <v>1.4999999999999999E-4</v>
       </c>
-      <c r="L7" s="2"/>
+      <c r="L7" s="3"/>
       <c r="M7">
         <v>500</v>
       </c>
@@ -1799,8 +2289,23 @@
         <f t="array" ref="S7">_xlfn.STDEV.S((H155:H184)*0.00001)</f>
         <v>2.795718900439597E-3</v>
       </c>
-    </row>
-    <row r="8" spans="3:19" x14ac:dyDescent="0.25">
+      <c r="V7" t="s">
+        <v>0</v>
+      </c>
+      <c r="W7">
+        <v>100</v>
+      </c>
+      <c r="X7" t="s">
+        <v>2</v>
+      </c>
+      <c r="Y7">
+        <v>8.0000000000000002E-3</v>
+      </c>
+      <c r="Z7" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="8" spans="3:26" x14ac:dyDescent="0.25">
       <c r="C8" t="s">
         <v>0</v>
       </c>
@@ -1825,7 +2330,7 @@
       <c r="J8">
         <v>1.4999999999999999E-4</v>
       </c>
-      <c r="L8" s="2"/>
+      <c r="L8" s="3"/>
       <c r="M8">
         <v>1000</v>
       </c>
@@ -1853,8 +2358,23 @@
         <f t="array" ref="S8">_xlfn.STDEV.S((H245:H274)*0.00001)</f>
         <v>4.0683287497980707E-4</v>
       </c>
-    </row>
-    <row r="9" spans="3:19" x14ac:dyDescent="0.25">
+      <c r="V8" t="s">
+        <v>0</v>
+      </c>
+      <c r="W8">
+        <v>100</v>
+      </c>
+      <c r="X8" t="s">
+        <v>2</v>
+      </c>
+      <c r="Y8">
+        <v>8.0000000000000002E-3</v>
+      </c>
+      <c r="Z8" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="9" spans="3:26" x14ac:dyDescent="0.25">
       <c r="C9" t="s">
         <v>0</v>
       </c>
@@ -1879,8 +2399,23 @@
       <c r="J9">
         <v>1.4999999999999999E-4</v>
       </c>
-    </row>
-    <row r="10" spans="3:19" x14ac:dyDescent="0.25">
+      <c r="V9" t="s">
+        <v>0</v>
+      </c>
+      <c r="W9">
+        <v>100</v>
+      </c>
+      <c r="X9" t="s">
+        <v>2</v>
+      </c>
+      <c r="Y9">
+        <v>7.0000000000000001E-3</v>
+      </c>
+      <c r="Z9" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="10" spans="3:26" x14ac:dyDescent="0.25">
       <c r="C10" t="s">
         <v>0</v>
       </c>
@@ -1905,8 +2440,23 @@
       <c r="J10">
         <v>1.4999999999999999E-4</v>
       </c>
-    </row>
-    <row r="11" spans="3:19" x14ac:dyDescent="0.25">
+      <c r="V10" t="s">
+        <v>0</v>
+      </c>
+      <c r="W10">
+        <v>100</v>
+      </c>
+      <c r="X10" t="s">
+        <v>2</v>
+      </c>
+      <c r="Y10">
+        <v>7.0000000000000001E-3</v>
+      </c>
+      <c r="Z10" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="11" spans="3:26" x14ac:dyDescent="0.25">
       <c r="C11" t="s">
         <v>0</v>
       </c>
@@ -1931,11 +2481,35 @@
       <c r="J11">
         <v>1.4999999999999999E-4</v>
       </c>
+      <c r="M11" t="s">
+        <v>4</v>
+      </c>
+      <c r="N11" t="s">
+        <v>7</v>
+      </c>
       <c r="O11" t="s">
         <v>8</v>
       </c>
-    </row>
-    <row r="12" spans="3:19" x14ac:dyDescent="0.25">
+      <c r="P11" t="s">
+        <v>22</v>
+      </c>
+      <c r="V11" t="s">
+        <v>0</v>
+      </c>
+      <c r="W11">
+        <v>100</v>
+      </c>
+      <c r="X11" t="s">
+        <v>2</v>
+      </c>
+      <c r="Y11">
+        <v>7.0000000000000001E-3</v>
+      </c>
+      <c r="Z11" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="12" spans="3:26" x14ac:dyDescent="0.25">
       <c r="C12" t="s">
         <v>0</v>
       </c>
@@ -1966,8 +2540,31 @@
       <c r="N12">
         <v>12</v>
       </c>
-    </row>
-    <row r="13" spans="3:19" x14ac:dyDescent="0.25">
+      <c r="O12">
+        <f>N39/N6</f>
+        <v>0.63806986538109001</v>
+      </c>
+      <c r="P12">
+        <f>O12/N12</f>
+        <v>5.3172488781757503E-2</v>
+      </c>
+      <c r="V12" t="s">
+        <v>0</v>
+      </c>
+      <c r="W12">
+        <v>100</v>
+      </c>
+      <c r="X12" t="s">
+        <v>2</v>
+      </c>
+      <c r="Y12">
+        <v>7.0000000000000001E-3</v>
+      </c>
+      <c r="Z12" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="13" spans="3:26" x14ac:dyDescent="0.25">
       <c r="C13" t="s">
         <v>0</v>
       </c>
@@ -1992,11 +2589,37 @@
       <c r="J13">
         <v>1.4999999999999999E-4</v>
       </c>
+      <c r="M13">
+        <v>0</v>
+      </c>
       <c r="N13">
         <v>50</v>
       </c>
-    </row>
-    <row r="14" spans="3:19" x14ac:dyDescent="0.25">
+      <c r="O13">
+        <f>N39/P6</f>
+        <v>0.36447200371833399</v>
+      </c>
+      <c r="P13">
+        <f t="shared" ref="P13:P20" si="0">O13/N13</f>
+        <v>7.2894400743666798E-3</v>
+      </c>
+      <c r="V13" t="s">
+        <v>0</v>
+      </c>
+      <c r="W13">
+        <v>100</v>
+      </c>
+      <c r="X13" t="s">
+        <v>2</v>
+      </c>
+      <c r="Y13">
+        <v>7.0000000000000001E-3</v>
+      </c>
+      <c r="Z13" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="14" spans="3:26" x14ac:dyDescent="0.25">
       <c r="C14" t="s">
         <v>0</v>
       </c>
@@ -2021,11 +2644,37 @@
       <c r="J14">
         <v>1.4999999999999999E-4</v>
       </c>
+      <c r="M14">
+        <v>0</v>
+      </c>
       <c r="N14">
         <v>100</v>
       </c>
-    </row>
-    <row r="15" spans="3:19" x14ac:dyDescent="0.25">
+      <c r="O14">
+        <f>N39/R6</f>
+        <v>4.1282891526095667E-3</v>
+      </c>
+      <c r="P14">
+        <f t="shared" si="0"/>
+        <v>4.1282891526095666E-5</v>
+      </c>
+      <c r="V14" t="s">
+        <v>0</v>
+      </c>
+      <c r="W14">
+        <v>100</v>
+      </c>
+      <c r="X14" t="s">
+        <v>2</v>
+      </c>
+      <c r="Y14">
+        <v>8.0000000000000002E-3</v>
+      </c>
+      <c r="Z14" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="15" spans="3:26" x14ac:dyDescent="0.25">
       <c r="C15" t="s">
         <v>0</v>
       </c>
@@ -2056,8 +2705,31 @@
       <c r="N15">
         <v>12</v>
       </c>
-    </row>
-    <row r="16" spans="3:19" x14ac:dyDescent="0.25">
+      <c r="O15">
+        <f>N40/N7</f>
+        <v>38.545368403239365</v>
+      </c>
+      <c r="P15">
+        <f t="shared" si="0"/>
+        <v>3.2121140336032803</v>
+      </c>
+      <c r="V15" t="s">
+        <v>0</v>
+      </c>
+      <c r="W15">
+        <v>100</v>
+      </c>
+      <c r="X15" t="s">
+        <v>2</v>
+      </c>
+      <c r="Y15">
+        <v>8.0000000000000002E-3</v>
+      </c>
+      <c r="Z15" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="16" spans="3:26" x14ac:dyDescent="0.25">
       <c r="C16" t="s">
         <v>0</v>
       </c>
@@ -2082,11 +2754,37 @@
       <c r="J16">
         <v>1.6000000000000001E-4</v>
       </c>
+      <c r="M16">
+        <v>0</v>
+      </c>
       <c r="N16">
         <v>50</v>
       </c>
-    </row>
-    <row r="17" spans="3:14" x14ac:dyDescent="0.25">
+      <c r="O16">
+        <f>N40/P7</f>
+        <v>90.049203158267233</v>
+      </c>
+      <c r="P16">
+        <f t="shared" si="0"/>
+        <v>1.8009840631653447</v>
+      </c>
+      <c r="V16" t="s">
+        <v>0</v>
+      </c>
+      <c r="W16">
+        <v>100</v>
+      </c>
+      <c r="X16" t="s">
+        <v>2</v>
+      </c>
+      <c r="Y16">
+        <v>8.0000000000000002E-3</v>
+      </c>
+      <c r="Z16" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="17" spans="3:26" x14ac:dyDescent="0.25">
       <c r="C17" t="s">
         <v>0</v>
       </c>
@@ -2111,11 +2809,37 @@
       <c r="J17">
         <v>1.6000000000000001E-4</v>
       </c>
+      <c r="M17">
+        <v>0</v>
+      </c>
       <c r="N17">
         <v>100</v>
       </c>
-    </row>
-    <row r="18" spans="3:14" x14ac:dyDescent="0.25">
+      <c r="O17">
+        <f>N40/R7</f>
+        <v>45.709790697341226</v>
+      </c>
+      <c r="P17">
+        <f t="shared" si="0"/>
+        <v>0.45709790697341224</v>
+      </c>
+      <c r="V17" t="s">
+        <v>0</v>
+      </c>
+      <c r="W17">
+        <v>100</v>
+      </c>
+      <c r="X17" t="s">
+        <v>2</v>
+      </c>
+      <c r="Y17">
+        <v>7.0000000000000001E-3</v>
+      </c>
+      <c r="Z17" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="18" spans="3:26" x14ac:dyDescent="0.25">
       <c r="C18" t="s">
         <v>0</v>
       </c>
@@ -2146,8 +2870,31 @@
       <c r="N18">
         <v>12</v>
       </c>
-    </row>
-    <row r="19" spans="3:14" x14ac:dyDescent="0.25">
+      <c r="O18">
+        <f>N41/N8</f>
+        <v>59.482466870010633</v>
+      </c>
+      <c r="P18">
+        <f t="shared" si="0"/>
+        <v>4.956872239167553</v>
+      </c>
+      <c r="V18" t="s">
+        <v>0</v>
+      </c>
+      <c r="W18">
+        <v>100</v>
+      </c>
+      <c r="X18" t="s">
+        <v>2</v>
+      </c>
+      <c r="Y18">
+        <v>7.0000000000000001E-3</v>
+      </c>
+      <c r="Z18" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="19" spans="3:26" x14ac:dyDescent="0.25">
       <c r="C19" t="s">
         <v>0</v>
       </c>
@@ -2172,11 +2919,37 @@
       <c r="J19">
         <v>1.6000000000000001E-4</v>
       </c>
+      <c r="M19">
+        <v>0</v>
+      </c>
       <c r="N19">
         <v>50</v>
       </c>
-    </row>
-    <row r="20" spans="3:14" x14ac:dyDescent="0.25">
+      <c r="O19">
+        <f>N41/P8</f>
+        <v>177.55767170644958</v>
+      </c>
+      <c r="P19">
+        <f t="shared" si="0"/>
+        <v>3.5511534341289916</v>
+      </c>
+      <c r="V19" t="s">
+        <v>0</v>
+      </c>
+      <c r="W19">
+        <v>100</v>
+      </c>
+      <c r="X19" t="s">
+        <v>2</v>
+      </c>
+      <c r="Y19">
+        <v>8.0000000000000002E-3</v>
+      </c>
+      <c r="Z19" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="20" spans="3:26" x14ac:dyDescent="0.25">
       <c r="C20" t="s">
         <v>0</v>
       </c>
@@ -2201,11 +2974,37 @@
       <c r="J20">
         <v>1.6000000000000001E-4</v>
       </c>
+      <c r="M20">
+        <v>0</v>
+      </c>
       <c r="N20">
         <v>100</v>
       </c>
-    </row>
-    <row r="21" spans="3:14" x14ac:dyDescent="0.25">
+      <c r="O20">
+        <f>N41/R8</f>
+        <v>236.7436226246484</v>
+      </c>
+      <c r="P20">
+        <f t="shared" si="0"/>
+        <v>2.3674362262464839</v>
+      </c>
+      <c r="V20" t="s">
+        <v>0</v>
+      </c>
+      <c r="W20">
+        <v>100</v>
+      </c>
+      <c r="X20" t="s">
+        <v>2</v>
+      </c>
+      <c r="Y20">
+        <v>8.0000000000000002E-3</v>
+      </c>
+      <c r="Z20" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="21" spans="3:26" x14ac:dyDescent="0.25">
       <c r="C21" t="s">
         <v>0</v>
       </c>
@@ -2230,8 +3029,23 @@
       <c r="J21">
         <v>1.6000000000000001E-4</v>
       </c>
-    </row>
-    <row r="22" spans="3:14" x14ac:dyDescent="0.25">
+      <c r="V21" t="s">
+        <v>0</v>
+      </c>
+      <c r="W21">
+        <v>100</v>
+      </c>
+      <c r="X21" t="s">
+        <v>2</v>
+      </c>
+      <c r="Y21">
+        <v>8.0000000000000002E-3</v>
+      </c>
+      <c r="Z21" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="22" spans="3:26" x14ac:dyDescent="0.25">
       <c r="C22" t="s">
         <v>0</v>
       </c>
@@ -2256,8 +3070,23 @@
       <c r="J22">
         <v>1.6000000000000001E-4</v>
       </c>
-    </row>
-    <row r="23" spans="3:14" x14ac:dyDescent="0.25">
+      <c r="V22" t="s">
+        <v>0</v>
+      </c>
+      <c r="W22">
+        <v>100</v>
+      </c>
+      <c r="X22" t="s">
+        <v>2</v>
+      </c>
+      <c r="Y22">
+        <v>8.0000000000000002E-3</v>
+      </c>
+      <c r="Z22" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="23" spans="3:26" x14ac:dyDescent="0.25">
       <c r="C23" t="s">
         <v>0</v>
       </c>
@@ -2282,8 +3111,23 @@
       <c r="J23">
         <v>1.6000000000000001E-4</v>
       </c>
-    </row>
-    <row r="24" spans="3:14" x14ac:dyDescent="0.25">
+      <c r="V23" t="s">
+        <v>0</v>
+      </c>
+      <c r="W23">
+        <v>100</v>
+      </c>
+      <c r="X23" t="s">
+        <v>2</v>
+      </c>
+      <c r="Y23">
+        <v>8.0000000000000002E-3</v>
+      </c>
+      <c r="Z23" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="24" spans="3:26" x14ac:dyDescent="0.25">
       <c r="C24" t="s">
         <v>0</v>
       </c>
@@ -2308,8 +3152,23 @@
       <c r="J24">
         <v>1.6000000000000001E-4</v>
       </c>
-    </row>
-    <row r="25" spans="3:14" x14ac:dyDescent="0.25">
+      <c r="V24" t="s">
+        <v>0</v>
+      </c>
+      <c r="W24">
+        <v>100</v>
+      </c>
+      <c r="X24" t="s">
+        <v>2</v>
+      </c>
+      <c r="Y24">
+        <v>8.0000000000000002E-3</v>
+      </c>
+      <c r="Z24" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="25" spans="3:26" x14ac:dyDescent="0.25">
       <c r="C25" t="s">
         <v>0</v>
       </c>
@@ -2334,8 +3193,23 @@
       <c r="J25">
         <v>1.4999999999999999E-4</v>
       </c>
-    </row>
-    <row r="26" spans="3:14" x14ac:dyDescent="0.25">
+      <c r="V25" t="s">
+        <v>0</v>
+      </c>
+      <c r="W25">
+        <v>100</v>
+      </c>
+      <c r="X25" t="s">
+        <v>2</v>
+      </c>
+      <c r="Y25">
+        <v>8.0000000000000002E-3</v>
+      </c>
+      <c r="Z25" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="26" spans="3:26" x14ac:dyDescent="0.25">
       <c r="C26" t="s">
         <v>0</v>
       </c>
@@ -2360,8 +3234,23 @@
       <c r="J26">
         <v>1.4999999999999999E-4</v>
       </c>
-    </row>
-    <row r="27" spans="3:14" x14ac:dyDescent="0.25">
+      <c r="V26" t="s">
+        <v>0</v>
+      </c>
+      <c r="W26">
+        <v>100</v>
+      </c>
+      <c r="X26" t="s">
+        <v>2</v>
+      </c>
+      <c r="Y26">
+        <v>8.0000000000000002E-3</v>
+      </c>
+      <c r="Z26" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="27" spans="3:26" x14ac:dyDescent="0.25">
       <c r="C27" t="s">
         <v>0</v>
       </c>
@@ -2386,8 +3275,23 @@
       <c r="J27">
         <v>1.4999999999999999E-4</v>
       </c>
-    </row>
-    <row r="28" spans="3:14" x14ac:dyDescent="0.25">
+      <c r="V27" t="s">
+        <v>0</v>
+      </c>
+      <c r="W27">
+        <v>100</v>
+      </c>
+      <c r="X27" t="s">
+        <v>2</v>
+      </c>
+      <c r="Y27">
+        <v>8.9999999999999993E-3</v>
+      </c>
+      <c r="Z27" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="28" spans="3:26" x14ac:dyDescent="0.25">
       <c r="C28" t="s">
         <v>0</v>
       </c>
@@ -2412,8 +3316,23 @@
       <c r="J28">
         <v>1.4999999999999999E-4</v>
       </c>
-    </row>
-    <row r="29" spans="3:14" x14ac:dyDescent="0.25">
+      <c r="V28" t="s">
+        <v>0</v>
+      </c>
+      <c r="W28">
+        <v>100</v>
+      </c>
+      <c r="X28" t="s">
+        <v>2</v>
+      </c>
+      <c r="Y28">
+        <v>8.9999999999999993E-3</v>
+      </c>
+      <c r="Z28" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="29" spans="3:26" x14ac:dyDescent="0.25">
       <c r="C29" t="s">
         <v>0</v>
       </c>
@@ -2438,8 +3357,23 @@
       <c r="J29">
         <v>1.4999999999999999E-4</v>
       </c>
-    </row>
-    <row r="30" spans="3:14" x14ac:dyDescent="0.25">
+      <c r="V29" t="s">
+        <v>0</v>
+      </c>
+      <c r="W29">
+        <v>100</v>
+      </c>
+      <c r="X29" t="s">
+        <v>2</v>
+      </c>
+      <c r="Y29">
+        <v>8.9999999999999993E-3</v>
+      </c>
+      <c r="Z29" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="30" spans="3:26" x14ac:dyDescent="0.25">
       <c r="C30" t="s">
         <v>0</v>
       </c>
@@ -2464,8 +3398,23 @@
       <c r="J30">
         <v>1.4999999999999999E-4</v>
       </c>
-    </row>
-    <row r="31" spans="3:14" x14ac:dyDescent="0.25">
+      <c r="V30" t="s">
+        <v>0</v>
+      </c>
+      <c r="W30">
+        <v>100</v>
+      </c>
+      <c r="X30" t="s">
+        <v>2</v>
+      </c>
+      <c r="Y30">
+        <v>8.9999999999999993E-3</v>
+      </c>
+      <c r="Z30" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="31" spans="3:26" x14ac:dyDescent="0.25">
       <c r="C31" t="s">
         <v>0</v>
       </c>
@@ -2490,8 +3439,23 @@
       <c r="J31">
         <v>1.4999999999999999E-4</v>
       </c>
-    </row>
-    <row r="32" spans="3:14" x14ac:dyDescent="0.25">
+      <c r="V31" t="s">
+        <v>0</v>
+      </c>
+      <c r="W31">
+        <v>100</v>
+      </c>
+      <c r="X31" t="s">
+        <v>2</v>
+      </c>
+      <c r="Y31">
+        <v>8.9999999999999993E-3</v>
+      </c>
+      <c r="Z31" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="32" spans="3:26" x14ac:dyDescent="0.25">
       <c r="C32" t="s">
         <v>0</v>
       </c>
@@ -2516,8 +3480,23 @@
       <c r="J32">
         <v>1.4999999999999999E-4</v>
       </c>
-    </row>
-    <row r="33" spans="3:10" x14ac:dyDescent="0.25">
+      <c r="V32" t="s">
+        <v>0</v>
+      </c>
+      <c r="W32">
+        <v>100</v>
+      </c>
+      <c r="X32" t="s">
+        <v>2</v>
+      </c>
+      <c r="Y32">
+        <v>8.0000000000000002E-3</v>
+      </c>
+      <c r="Z32" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="33" spans="3:26" x14ac:dyDescent="0.25">
       <c r="C33" t="s">
         <v>0</v>
       </c>
@@ -2542,8 +3521,23 @@
       <c r="J33">
         <v>1.4999999999999999E-4</v>
       </c>
-    </row>
-    <row r="34" spans="3:10" x14ac:dyDescent="0.25">
+      <c r="V33" t="s">
+        <v>0</v>
+      </c>
+      <c r="W33">
+        <v>100</v>
+      </c>
+      <c r="X33" t="s">
+        <v>2</v>
+      </c>
+      <c r="Y33">
+        <v>8.0000000000000002E-3</v>
+      </c>
+      <c r="Z33" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="34" spans="3:26" x14ac:dyDescent="0.25">
       <c r="C34" t="s">
         <v>0</v>
       </c>
@@ -2568,8 +3562,23 @@
       <c r="J34">
         <v>1.4999999999999999E-4</v>
       </c>
-    </row>
-    <row r="35" spans="3:10" x14ac:dyDescent="0.25">
+      <c r="V34" t="s">
+        <v>0</v>
+      </c>
+      <c r="W34">
+        <v>100</v>
+      </c>
+      <c r="X34" t="s">
+        <v>2</v>
+      </c>
+      <c r="Y34">
+        <v>8.0000000000000002E-3</v>
+      </c>
+      <c r="Z34" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="35" spans="3:26" x14ac:dyDescent="0.25">
       <c r="C35" t="s">
         <v>0</v>
       </c>
@@ -2594,8 +3603,23 @@
       <c r="J35">
         <v>3.8999999999999999E-4</v>
       </c>
-    </row>
-    <row r="36" spans="3:10" x14ac:dyDescent="0.25">
+      <c r="V35" t="s">
+        <v>0</v>
+      </c>
+      <c r="W35">
+        <v>500</v>
+      </c>
+      <c r="X35" t="s">
+        <v>2</v>
+      </c>
+      <c r="Y35">
+        <v>1.2849999999999999</v>
+      </c>
+      <c r="Z35" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="36" spans="3:26" x14ac:dyDescent="0.25">
       <c r="C36" t="s">
         <v>0</v>
       </c>
@@ -2620,8 +3644,23 @@
       <c r="J36">
         <v>3.8999999999999999E-4</v>
       </c>
-    </row>
-    <row r="37" spans="3:10" x14ac:dyDescent="0.25">
+      <c r="V36" t="s">
+        <v>0</v>
+      </c>
+      <c r="W36">
+        <v>500</v>
+      </c>
+      <c r="X36" t="s">
+        <v>2</v>
+      </c>
+      <c r="Y36">
+        <v>1.2609999999999999</v>
+      </c>
+      <c r="Z36" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="37" spans="3:26" x14ac:dyDescent="0.25">
       <c r="C37" t="s">
         <v>0</v>
       </c>
@@ -2646,8 +3685,23 @@
       <c r="J37">
         <v>3.8999999999999999E-4</v>
       </c>
-    </row>
-    <row r="38" spans="3:10" x14ac:dyDescent="0.25">
+      <c r="V37" t="s">
+        <v>0</v>
+      </c>
+      <c r="W37">
+        <v>500</v>
+      </c>
+      <c r="X37" t="s">
+        <v>2</v>
+      </c>
+      <c r="Y37">
+        <v>1.3029999999999999</v>
+      </c>
+      <c r="Z37" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="38" spans="3:26" x14ac:dyDescent="0.25">
       <c r="C38" t="s">
         <v>0</v>
       </c>
@@ -2672,8 +3726,32 @@
       <c r="J38">
         <v>3.8999999999999999E-4</v>
       </c>
-    </row>
-    <row r="39" spans="3:10" x14ac:dyDescent="0.25">
+      <c r="M38" t="s">
+        <v>4</v>
+      </c>
+      <c r="N38" t="s">
+        <v>5</v>
+      </c>
+      <c r="O38" t="s">
+        <v>6</v>
+      </c>
+      <c r="V38" t="s">
+        <v>0</v>
+      </c>
+      <c r="W38">
+        <v>500</v>
+      </c>
+      <c r="X38" t="s">
+        <v>2</v>
+      </c>
+      <c r="Y38">
+        <v>1.3089999999999999</v>
+      </c>
+      <c r="Z38" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="39" spans="3:26" x14ac:dyDescent="0.25">
       <c r="C39" t="s">
         <v>0</v>
       </c>
@@ -2698,8 +3776,34 @@
       <c r="J39">
         <v>3.8999999999999999E-4</v>
       </c>
-    </row>
-    <row r="40" spans="3:10" x14ac:dyDescent="0.25">
+      <c r="M39">
+        <v>100</v>
+      </c>
+      <c r="N39">
+        <f>SUMIFS($Y:$Y,$W:$W,$M39)/30</f>
+        <v>7.9333333333333391E-3</v>
+      </c>
+      <c r="O39">
+        <f>_xlfn.STDEV.S(Y5:Y34)</f>
+        <v>6.3968382994949156E-4</v>
+      </c>
+      <c r="V39" t="s">
+        <v>0</v>
+      </c>
+      <c r="W39">
+        <v>500</v>
+      </c>
+      <c r="X39" t="s">
+        <v>2</v>
+      </c>
+      <c r="Y39">
+        <v>1.262</v>
+      </c>
+      <c r="Z39" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="40" spans="3:26" x14ac:dyDescent="0.25">
       <c r="C40" t="s">
         <v>0</v>
       </c>
@@ -2724,8 +3828,34 @@
       <c r="J40">
         <v>3.8999999999999999E-4</v>
       </c>
-    </row>
-    <row r="41" spans="3:10" x14ac:dyDescent="0.25">
+      <c r="M40">
+        <v>500</v>
+      </c>
+      <c r="N40">
+        <f>SUMIFS($Y:$Y,$W:$W,$M40)/30</f>
+        <v>1.4017666666666668</v>
+      </c>
+      <c r="O40">
+        <f>_xlfn.STDEV.S(Y35:Y64)</f>
+        <v>0.16944914471214478</v>
+      </c>
+      <c r="V40" t="s">
+        <v>0</v>
+      </c>
+      <c r="W40">
+        <v>500</v>
+      </c>
+      <c r="X40" t="s">
+        <v>2</v>
+      </c>
+      <c r="Y40">
+        <v>1.3779999999999999</v>
+      </c>
+      <c r="Z40" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="41" spans="3:26" x14ac:dyDescent="0.25">
       <c r="C41" t="s">
         <v>0</v>
       </c>
@@ -2750,8 +3880,34 @@
       <c r="J41">
         <v>3.8999999999999999E-4</v>
       </c>
-    </row>
-    <row r="42" spans="3:10" x14ac:dyDescent="0.25">
+      <c r="M41">
+        <v>1000</v>
+      </c>
+      <c r="N41">
+        <f>SUMIFS($Y:$Y,$W:$W,$M41)/30</f>
+        <v>11.079599999999999</v>
+      </c>
+      <c r="O41">
+        <f>_xlfn.STDEV.S(Y65:Y94)</f>
+        <v>0.42670530895414838</v>
+      </c>
+      <c r="V41" t="s">
+        <v>0</v>
+      </c>
+      <c r="W41">
+        <v>500</v>
+      </c>
+      <c r="X41" t="s">
+        <v>2</v>
+      </c>
+      <c r="Y41">
+        <v>1.337</v>
+      </c>
+      <c r="Z41" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="42" spans="3:26" x14ac:dyDescent="0.25">
       <c r="C42" t="s">
         <v>0</v>
       </c>
@@ -2776,8 +3932,23 @@
       <c r="J42">
         <v>3.8999999999999999E-4</v>
       </c>
-    </row>
-    <row r="43" spans="3:10" x14ac:dyDescent="0.25">
+      <c r="V42" t="s">
+        <v>0</v>
+      </c>
+      <c r="W42">
+        <v>500</v>
+      </c>
+      <c r="X42" t="s">
+        <v>2</v>
+      </c>
+      <c r="Y42">
+        <v>1.2869999999999999</v>
+      </c>
+      <c r="Z42" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="43" spans="3:26" x14ac:dyDescent="0.25">
       <c r="C43" t="s">
         <v>0</v>
       </c>
@@ -2802,8 +3973,23 @@
       <c r="J43">
         <v>3.8999999999999999E-4</v>
       </c>
-    </row>
-    <row r="44" spans="3:10" x14ac:dyDescent="0.25">
+      <c r="V43" t="s">
+        <v>0</v>
+      </c>
+      <c r="W43">
+        <v>500</v>
+      </c>
+      <c r="X43" t="s">
+        <v>2</v>
+      </c>
+      <c r="Y43">
+        <v>1.3149999999999999</v>
+      </c>
+      <c r="Z43" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="44" spans="3:26" x14ac:dyDescent="0.25">
       <c r="C44" t="s">
         <v>0</v>
       </c>
@@ -2828,8 +4014,23 @@
       <c r="J44">
         <v>3.8999999999999999E-4</v>
       </c>
-    </row>
-    <row r="45" spans="3:10" x14ac:dyDescent="0.25">
+      <c r="V44" t="s">
+        <v>0</v>
+      </c>
+      <c r="W44">
+        <v>500</v>
+      </c>
+      <c r="X44" t="s">
+        <v>2</v>
+      </c>
+      <c r="Y44">
+        <v>1.4330000000000001</v>
+      </c>
+      <c r="Z44" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="45" spans="3:26" x14ac:dyDescent="0.25">
       <c r="C45" t="s">
         <v>0</v>
       </c>
@@ -2854,8 +4055,23 @@
       <c r="J45">
         <v>3.8999999999999999E-4</v>
       </c>
-    </row>
-    <row r="46" spans="3:10" x14ac:dyDescent="0.25">
+      <c r="V45" t="s">
+        <v>0</v>
+      </c>
+      <c r="W45">
+        <v>500</v>
+      </c>
+      <c r="X45" t="s">
+        <v>2</v>
+      </c>
+      <c r="Y45">
+        <v>1.5820000000000001</v>
+      </c>
+      <c r="Z45" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="46" spans="3:26" x14ac:dyDescent="0.25">
       <c r="C46" t="s">
         <v>0</v>
       </c>
@@ -2880,8 +4096,23 @@
       <c r="J46">
         <v>3.8999999999999999E-4</v>
       </c>
-    </row>
-    <row r="47" spans="3:10" x14ac:dyDescent="0.25">
+      <c r="V46" t="s">
+        <v>0</v>
+      </c>
+      <c r="W46">
+        <v>500</v>
+      </c>
+      <c r="X46" t="s">
+        <v>2</v>
+      </c>
+      <c r="Y46">
+        <v>1.7230000000000001</v>
+      </c>
+      <c r="Z46" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="47" spans="3:26" x14ac:dyDescent="0.25">
       <c r="C47" t="s">
         <v>0</v>
       </c>
@@ -2906,8 +4137,23 @@
       <c r="J47">
         <v>3.8999999999999999E-4</v>
       </c>
-    </row>
-    <row r="48" spans="3:10" x14ac:dyDescent="0.25">
+      <c r="V47" t="s">
+        <v>0</v>
+      </c>
+      <c r="W47">
+        <v>500</v>
+      </c>
+      <c r="X47" t="s">
+        <v>2</v>
+      </c>
+      <c r="Y47">
+        <v>1.355</v>
+      </c>
+      <c r="Z47" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="48" spans="3:26" x14ac:dyDescent="0.25">
       <c r="C48" t="s">
         <v>0</v>
       </c>
@@ -2932,8 +4178,23 @@
       <c r="J48">
         <v>4.0000000000000002E-4</v>
       </c>
-    </row>
-    <row r="49" spans="3:10" x14ac:dyDescent="0.25">
+      <c r="V48" t="s">
+        <v>0</v>
+      </c>
+      <c r="W48">
+        <v>500</v>
+      </c>
+      <c r="X48" t="s">
+        <v>2</v>
+      </c>
+      <c r="Y48">
+        <v>1.4059999999999999</v>
+      </c>
+      <c r="Z48" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="49" spans="3:26" x14ac:dyDescent="0.25">
       <c r="C49" t="s">
         <v>0</v>
       </c>
@@ -2958,8 +4219,23 @@
       <c r="J49">
         <v>4.0000000000000002E-4</v>
       </c>
-    </row>
-    <row r="50" spans="3:10" x14ac:dyDescent="0.25">
+      <c r="V49" t="s">
+        <v>0</v>
+      </c>
+      <c r="W49">
+        <v>500</v>
+      </c>
+      <c r="X49" t="s">
+        <v>2</v>
+      </c>
+      <c r="Y49">
+        <v>1.341</v>
+      </c>
+      <c r="Z49" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="50" spans="3:26" x14ac:dyDescent="0.25">
       <c r="C50" t="s">
         <v>0</v>
       </c>
@@ -2984,8 +4260,23 @@
       <c r="J50">
         <v>4.0000000000000002E-4</v>
       </c>
-    </row>
-    <row r="51" spans="3:10" x14ac:dyDescent="0.25">
+      <c r="V50" t="s">
+        <v>0</v>
+      </c>
+      <c r="W50">
+        <v>500</v>
+      </c>
+      <c r="X50" t="s">
+        <v>2</v>
+      </c>
+      <c r="Y50">
+        <v>1.256</v>
+      </c>
+      <c r="Z50" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="51" spans="3:26" x14ac:dyDescent="0.25">
       <c r="C51" t="s">
         <v>0</v>
       </c>
@@ -3010,8 +4301,23 @@
       <c r="J51">
         <v>4.0000000000000002E-4</v>
       </c>
-    </row>
-    <row r="52" spans="3:10" x14ac:dyDescent="0.25">
+      <c r="V51" t="s">
+        <v>0</v>
+      </c>
+      <c r="W51">
+        <v>500</v>
+      </c>
+      <c r="X51" t="s">
+        <v>2</v>
+      </c>
+      <c r="Y51">
+        <v>1.331</v>
+      </c>
+      <c r="Z51" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="52" spans="3:26" x14ac:dyDescent="0.25">
       <c r="C52" t="s">
         <v>0</v>
       </c>
@@ -3036,8 +4342,23 @@
       <c r="J52">
         <v>4.0000000000000002E-4</v>
       </c>
-    </row>
-    <row r="53" spans="3:10" x14ac:dyDescent="0.25">
+      <c r="V52" t="s">
+        <v>0</v>
+      </c>
+      <c r="W52">
+        <v>500</v>
+      </c>
+      <c r="X52" t="s">
+        <v>2</v>
+      </c>
+      <c r="Y52">
+        <v>1.2969999999999999</v>
+      </c>
+      <c r="Z52" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="53" spans="3:26" x14ac:dyDescent="0.25">
       <c r="C53" t="s">
         <v>0</v>
       </c>
@@ -3062,8 +4383,23 @@
       <c r="J53">
         <v>4.0000000000000002E-4</v>
       </c>
-    </row>
-    <row r="54" spans="3:10" x14ac:dyDescent="0.25">
+      <c r="V53" t="s">
+        <v>0</v>
+      </c>
+      <c r="W53">
+        <v>500</v>
+      </c>
+      <c r="X53" t="s">
+        <v>2</v>
+      </c>
+      <c r="Y53">
+        <v>1.742</v>
+      </c>
+      <c r="Z53" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="54" spans="3:26" x14ac:dyDescent="0.25">
       <c r="C54" t="s">
         <v>0</v>
       </c>
@@ -3088,8 +4424,23 @@
       <c r="J54">
         <v>4.0000000000000002E-4</v>
       </c>
-    </row>
-    <row r="55" spans="3:10" x14ac:dyDescent="0.25">
+      <c r="V54" t="s">
+        <v>0</v>
+      </c>
+      <c r="W54">
+        <v>500</v>
+      </c>
+      <c r="X54" t="s">
+        <v>2</v>
+      </c>
+      <c r="Y54">
+        <v>1.4079999999999999</v>
+      </c>
+      <c r="Z54" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="55" spans="3:26" x14ac:dyDescent="0.25">
       <c r="C55" t="s">
         <v>0</v>
       </c>
@@ -3114,8 +4465,23 @@
       <c r="J55">
         <v>4.0000000000000002E-4</v>
       </c>
-    </row>
-    <row r="56" spans="3:10" x14ac:dyDescent="0.25">
+      <c r="V55" t="s">
+        <v>0</v>
+      </c>
+      <c r="W55">
+        <v>500</v>
+      </c>
+      <c r="X55" t="s">
+        <v>2</v>
+      </c>
+      <c r="Y55">
+        <v>1.6539999999999999</v>
+      </c>
+      <c r="Z55" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="56" spans="3:26" x14ac:dyDescent="0.25">
       <c r="C56" t="s">
         <v>0</v>
       </c>
@@ -3140,8 +4506,23 @@
       <c r="J56">
         <v>4.0000000000000002E-4</v>
       </c>
-    </row>
-    <row r="57" spans="3:10" x14ac:dyDescent="0.25">
+      <c r="V56" t="s">
+        <v>0</v>
+      </c>
+      <c r="W56">
+        <v>500</v>
+      </c>
+      <c r="X56" t="s">
+        <v>2</v>
+      </c>
+      <c r="Y56">
+        <v>1.972</v>
+      </c>
+      <c r="Z56" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="57" spans="3:26" x14ac:dyDescent="0.25">
       <c r="C57" t="s">
         <v>0</v>
       </c>
@@ -3166,8 +4547,23 @@
       <c r="J57">
         <v>3.6999999999999999E-4</v>
       </c>
-    </row>
-    <row r="58" spans="3:10" x14ac:dyDescent="0.25">
+      <c r="V57" t="s">
+        <v>0</v>
+      </c>
+      <c r="W57">
+        <v>500</v>
+      </c>
+      <c r="X57" t="s">
+        <v>2</v>
+      </c>
+      <c r="Y57">
+        <v>1.429</v>
+      </c>
+      <c r="Z57" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="58" spans="3:26" x14ac:dyDescent="0.25">
       <c r="C58" t="s">
         <v>0</v>
       </c>
@@ -3192,8 +4588,23 @@
       <c r="J58">
         <v>3.6999999999999999E-4</v>
       </c>
-    </row>
-    <row r="59" spans="3:10" x14ac:dyDescent="0.25">
+      <c r="V58" t="s">
+        <v>0</v>
+      </c>
+      <c r="W58">
+        <v>500</v>
+      </c>
+      <c r="X58" t="s">
+        <v>2</v>
+      </c>
+      <c r="Y58">
+        <v>1.321</v>
+      </c>
+      <c r="Z58" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="59" spans="3:26" x14ac:dyDescent="0.25">
       <c r="C59" t="s">
         <v>0</v>
       </c>
@@ -3218,8 +4629,23 @@
       <c r="J59">
         <v>3.6999999999999999E-4</v>
       </c>
-    </row>
-    <row r="60" spans="3:10" x14ac:dyDescent="0.25">
+      <c r="V59" t="s">
+        <v>0</v>
+      </c>
+      <c r="W59">
+        <v>500</v>
+      </c>
+      <c r="X59" t="s">
+        <v>2</v>
+      </c>
+      <c r="Y59">
+        <v>1.335</v>
+      </c>
+      <c r="Z59" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="60" spans="3:26" x14ac:dyDescent="0.25">
       <c r="C60" t="s">
         <v>0</v>
       </c>
@@ -3244,8 +4670,23 @@
       <c r="J60">
         <v>3.6999999999999999E-4</v>
       </c>
-    </row>
-    <row r="61" spans="3:10" x14ac:dyDescent="0.25">
+      <c r="V60" t="s">
+        <v>0</v>
+      </c>
+      <c r="W60">
+        <v>500</v>
+      </c>
+      <c r="X60" t="s">
+        <v>2</v>
+      </c>
+      <c r="Y60">
+        <v>1.4019999999999999</v>
+      </c>
+      <c r="Z60" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="61" spans="3:26" x14ac:dyDescent="0.25">
       <c r="C61" t="s">
         <v>0</v>
       </c>
@@ -3270,8 +4711,23 @@
       <c r="J61">
         <v>3.6999999999999999E-4</v>
       </c>
-    </row>
-    <row r="62" spans="3:10" x14ac:dyDescent="0.25">
+      <c r="V61" t="s">
+        <v>0</v>
+      </c>
+      <c r="W61">
+        <v>500</v>
+      </c>
+      <c r="X61" t="s">
+        <v>2</v>
+      </c>
+      <c r="Y61">
+        <v>1.2709999999999999</v>
+      </c>
+      <c r="Z61" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="62" spans="3:26" x14ac:dyDescent="0.25">
       <c r="C62" t="s">
         <v>0</v>
       </c>
@@ -3296,8 +4752,23 @@
       <c r="J62">
         <v>3.6999999999999999E-4</v>
       </c>
-    </row>
-    <row r="63" spans="3:10" x14ac:dyDescent="0.25">
+      <c r="V62" t="s">
+        <v>0</v>
+      </c>
+      <c r="W62">
+        <v>500</v>
+      </c>
+      <c r="X62" t="s">
+        <v>2</v>
+      </c>
+      <c r="Y62">
+        <v>1.454</v>
+      </c>
+      <c r="Z62" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="63" spans="3:26" x14ac:dyDescent="0.25">
       <c r="C63" t="s">
         <v>0</v>
       </c>
@@ -3322,8 +4793,23 @@
       <c r="J63">
         <v>3.6999999999999999E-4</v>
       </c>
-    </row>
-    <row r="64" spans="3:10" x14ac:dyDescent="0.25">
+      <c r="V63" t="s">
+        <v>0</v>
+      </c>
+      <c r="W63">
+        <v>500</v>
+      </c>
+      <c r="X63" t="s">
+        <v>2</v>
+      </c>
+      <c r="Y63">
+        <v>1.3069999999999999</v>
+      </c>
+      <c r="Z63" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="64" spans="3:26" x14ac:dyDescent="0.25">
       <c r="C64" t="s">
         <v>0</v>
       </c>
@@ -3348,8 +4834,23 @@
       <c r="J64">
         <v>3.6999999999999999E-4</v>
       </c>
-    </row>
-    <row r="65" spans="3:10" x14ac:dyDescent="0.25">
+      <c r="V64" t="s">
+        <v>0</v>
+      </c>
+      <c r="W64">
+        <v>500</v>
+      </c>
+      <c r="X64" t="s">
+        <v>2</v>
+      </c>
+      <c r="Y64">
+        <v>1.2969999999999999</v>
+      </c>
+      <c r="Z64" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="65" spans="3:26" x14ac:dyDescent="0.25">
       <c r="C65" t="s">
         <v>0</v>
       </c>
@@ -3374,8 +4875,23 @@
       <c r="J65">
         <v>5.5000000000000003E-4</v>
       </c>
-    </row>
-    <row r="66" spans="3:10" x14ac:dyDescent="0.25">
+      <c r="V65" t="s">
+        <v>0</v>
+      </c>
+      <c r="W65">
+        <v>1000</v>
+      </c>
+      <c r="X65" t="s">
+        <v>2</v>
+      </c>
+      <c r="Y65">
+        <v>11.679</v>
+      </c>
+      <c r="Z65" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="66" spans="3:26" x14ac:dyDescent="0.25">
       <c r="C66" t="s">
         <v>0</v>
       </c>
@@ -3400,8 +4916,23 @@
       <c r="J66">
         <v>7.2000000000000005E-4</v>
       </c>
-    </row>
-    <row r="67" spans="3:10" x14ac:dyDescent="0.25">
+      <c r="V66" t="s">
+        <v>0</v>
+      </c>
+      <c r="W66">
+        <v>1000</v>
+      </c>
+      <c r="X66" t="s">
+        <v>2</v>
+      </c>
+      <c r="Y66">
+        <v>10.891</v>
+      </c>
+      <c r="Z66" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="67" spans="3:26" x14ac:dyDescent="0.25">
       <c r="C67" t="s">
         <v>0</v>
       </c>
@@ -3426,8 +4957,23 @@
       <c r="J67">
         <v>5.5000000000000003E-4</v>
       </c>
-    </row>
-    <row r="68" spans="3:10" x14ac:dyDescent="0.25">
+      <c r="V67" t="s">
+        <v>0</v>
+      </c>
+      <c r="W67">
+        <v>1000</v>
+      </c>
+      <c r="X67" t="s">
+        <v>2</v>
+      </c>
+      <c r="Y67">
+        <v>10.797000000000001</v>
+      </c>
+      <c r="Z67" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="68" spans="3:26" x14ac:dyDescent="0.25">
       <c r="C68" t="s">
         <v>0</v>
       </c>
@@ -3452,8 +4998,23 @@
       <c r="J68">
         <v>5.5000000000000003E-4</v>
       </c>
-    </row>
-    <row r="69" spans="3:10" x14ac:dyDescent="0.25">
+      <c r="V68" t="s">
+        <v>0</v>
+      </c>
+      <c r="W68">
+        <v>1000</v>
+      </c>
+      <c r="X68" t="s">
+        <v>2</v>
+      </c>
+      <c r="Y68">
+        <v>11.36</v>
+      </c>
+      <c r="Z68" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="69" spans="3:26" x14ac:dyDescent="0.25">
       <c r="C69" t="s">
         <v>0</v>
       </c>
@@ -3478,8 +5039,23 @@
       <c r="J69">
         <v>5.5000000000000003E-4</v>
       </c>
-    </row>
-    <row r="70" spans="3:10" x14ac:dyDescent="0.25">
+      <c r="V69" t="s">
+        <v>0</v>
+      </c>
+      <c r="W69">
+        <v>1000</v>
+      </c>
+      <c r="X69" t="s">
+        <v>2</v>
+      </c>
+      <c r="Y69">
+        <v>10.759</v>
+      </c>
+      <c r="Z69" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="70" spans="3:26" x14ac:dyDescent="0.25">
       <c r="C70" t="s">
         <v>0</v>
       </c>
@@ -3504,8 +5080,23 @@
       <c r="J70">
         <v>5.5000000000000003E-4</v>
       </c>
-    </row>
-    <row r="71" spans="3:10" x14ac:dyDescent="0.25">
+      <c r="V70" t="s">
+        <v>0</v>
+      </c>
+      <c r="W70">
+        <v>1000</v>
+      </c>
+      <c r="X70" t="s">
+        <v>2</v>
+      </c>
+      <c r="Y70">
+        <v>11.179</v>
+      </c>
+      <c r="Z70" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="71" spans="3:26" x14ac:dyDescent="0.25">
       <c r="C71" t="s">
         <v>0</v>
       </c>
@@ -3530,8 +5121,23 @@
       <c r="J71">
         <v>5.5000000000000003E-4</v>
       </c>
-    </row>
-    <row r="72" spans="3:10" x14ac:dyDescent="0.25">
+      <c r="V71" t="s">
+        <v>0</v>
+      </c>
+      <c r="W71">
+        <v>1000</v>
+      </c>
+      <c r="X71" t="s">
+        <v>2</v>
+      </c>
+      <c r="Y71">
+        <v>10.51</v>
+      </c>
+      <c r="Z71" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="72" spans="3:26" x14ac:dyDescent="0.25">
       <c r="C72" t="s">
         <v>0</v>
       </c>
@@ -3556,8 +5162,23 @@
       <c r="J72">
         <v>5.5000000000000003E-4</v>
       </c>
-    </row>
-    <row r="73" spans="3:10" x14ac:dyDescent="0.25">
+      <c r="V72" t="s">
+        <v>0</v>
+      </c>
+      <c r="W72">
+        <v>1000</v>
+      </c>
+      <c r="X72" t="s">
+        <v>2</v>
+      </c>
+      <c r="Y72">
+        <v>11.11</v>
+      </c>
+      <c r="Z72" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="73" spans="3:26" x14ac:dyDescent="0.25">
       <c r="C73" t="s">
         <v>0</v>
       </c>
@@ -3582,8 +5203,23 @@
       <c r="J73">
         <v>5.5000000000000003E-4</v>
       </c>
-    </row>
-    <row r="74" spans="3:10" x14ac:dyDescent="0.25">
+      <c r="V73" t="s">
+        <v>0</v>
+      </c>
+      <c r="W73">
+        <v>1000</v>
+      </c>
+      <c r="X73" t="s">
+        <v>2</v>
+      </c>
+      <c r="Y73">
+        <v>10.925000000000001</v>
+      </c>
+      <c r="Z73" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="74" spans="3:26" x14ac:dyDescent="0.25">
       <c r="C74" t="s">
         <v>0</v>
       </c>
@@ -3608,8 +5244,23 @@
       <c r="J74">
         <v>5.5000000000000003E-4</v>
       </c>
-    </row>
-    <row r="75" spans="3:10" x14ac:dyDescent="0.25">
+      <c r="V74" t="s">
+        <v>0</v>
+      </c>
+      <c r="W74">
+        <v>1000</v>
+      </c>
+      <c r="X74" t="s">
+        <v>2</v>
+      </c>
+      <c r="Y74">
+        <v>11.462</v>
+      </c>
+      <c r="Z74" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="75" spans="3:26" x14ac:dyDescent="0.25">
       <c r="C75" t="s">
         <v>0</v>
       </c>
@@ -3634,8 +5285,23 @@
       <c r="J75">
         <v>5.5000000000000003E-4</v>
       </c>
-    </row>
-    <row r="76" spans="3:10" x14ac:dyDescent="0.25">
+      <c r="V75" t="s">
+        <v>0</v>
+      </c>
+      <c r="W75">
+        <v>1000</v>
+      </c>
+      <c r="X75" t="s">
+        <v>2</v>
+      </c>
+      <c r="Y75">
+        <v>11.013</v>
+      </c>
+      <c r="Z75" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="76" spans="3:26" x14ac:dyDescent="0.25">
       <c r="C76" t="s">
         <v>0</v>
       </c>
@@ -3660,8 +5326,23 @@
       <c r="J76">
         <v>5.5000000000000003E-4</v>
       </c>
-    </row>
-    <row r="77" spans="3:10" x14ac:dyDescent="0.25">
+      <c r="V76" t="s">
+        <v>0</v>
+      </c>
+      <c r="W76">
+        <v>1000</v>
+      </c>
+      <c r="X76" t="s">
+        <v>2</v>
+      </c>
+      <c r="Y76">
+        <v>10.694000000000001</v>
+      </c>
+      <c r="Z76" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="77" spans="3:26" x14ac:dyDescent="0.25">
       <c r="C77" t="s">
         <v>0</v>
       </c>
@@ -3686,8 +5367,23 @@
       <c r="J77">
         <v>6.4999999999999997E-4</v>
       </c>
-    </row>
-    <row r="78" spans="3:10" x14ac:dyDescent="0.25">
+      <c r="V77" t="s">
+        <v>0</v>
+      </c>
+      <c r="W77">
+        <v>1000</v>
+      </c>
+      <c r="X77" t="s">
+        <v>2</v>
+      </c>
+      <c r="Y77">
+        <v>11.246</v>
+      </c>
+      <c r="Z77" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="78" spans="3:26" x14ac:dyDescent="0.25">
       <c r="C78" t="s">
         <v>0</v>
       </c>
@@ -3712,8 +5408,23 @@
       <c r="J78">
         <v>7.5000000000000002E-4</v>
       </c>
-    </row>
-    <row r="79" spans="3:10" x14ac:dyDescent="0.25">
+      <c r="V78" t="s">
+        <v>0</v>
+      </c>
+      <c r="W78">
+        <v>1000</v>
+      </c>
+      <c r="X78" t="s">
+        <v>2</v>
+      </c>
+      <c r="Y78">
+        <v>10.785</v>
+      </c>
+      <c r="Z78" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="79" spans="3:26" x14ac:dyDescent="0.25">
       <c r="C79" t="s">
         <v>0</v>
       </c>
@@ -3738,8 +5449,23 @@
       <c r="J79">
         <v>5.5000000000000003E-4</v>
       </c>
-    </row>
-    <row r="80" spans="3:10" x14ac:dyDescent="0.25">
+      <c r="V79" t="s">
+        <v>0</v>
+      </c>
+      <c r="W79">
+        <v>1000</v>
+      </c>
+      <c r="X79" t="s">
+        <v>2</v>
+      </c>
+      <c r="Y79">
+        <v>11.224</v>
+      </c>
+      <c r="Z79" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="80" spans="3:26" x14ac:dyDescent="0.25">
       <c r="C80" t="s">
         <v>0</v>
       </c>
@@ -3764,8 +5490,23 @@
       <c r="J80">
         <v>5.5000000000000003E-4</v>
       </c>
-    </row>
-    <row r="81" spans="3:10" x14ac:dyDescent="0.25">
+      <c r="V80" t="s">
+        <v>0</v>
+      </c>
+      <c r="W80">
+        <v>1000</v>
+      </c>
+      <c r="X80" t="s">
+        <v>2</v>
+      </c>
+      <c r="Y80">
+        <v>11.025</v>
+      </c>
+      <c r="Z80" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="81" spans="3:26" x14ac:dyDescent="0.25">
       <c r="C81" t="s">
         <v>0</v>
       </c>
@@ -3790,8 +5531,23 @@
       <c r="J81">
         <v>5.5000000000000003E-4</v>
       </c>
-    </row>
-    <row r="82" spans="3:10" x14ac:dyDescent="0.25">
+      <c r="V81" t="s">
+        <v>0</v>
+      </c>
+      <c r="W81">
+        <v>1000</v>
+      </c>
+      <c r="X81" t="s">
+        <v>2</v>
+      </c>
+      <c r="Y81">
+        <v>10.48</v>
+      </c>
+      <c r="Z81" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="82" spans="3:26" x14ac:dyDescent="0.25">
       <c r="C82" t="s">
         <v>0</v>
       </c>
@@ -3816,8 +5572,23 @@
       <c r="J82">
         <v>5.5000000000000003E-4</v>
       </c>
-    </row>
-    <row r="83" spans="3:10" x14ac:dyDescent="0.25">
+      <c r="V82" t="s">
+        <v>0</v>
+      </c>
+      <c r="W82">
+        <v>1000</v>
+      </c>
+      <c r="X82" t="s">
+        <v>2</v>
+      </c>
+      <c r="Y82">
+        <v>11.207000000000001</v>
+      </c>
+      <c r="Z82" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="83" spans="3:26" x14ac:dyDescent="0.25">
       <c r="C83" t="s">
         <v>0</v>
       </c>
@@ -3842,8 +5613,23 @@
       <c r="J83">
         <v>5.5000000000000003E-4</v>
       </c>
-    </row>
-    <row r="84" spans="3:10" x14ac:dyDescent="0.25">
+      <c r="V83" t="s">
+        <v>0</v>
+      </c>
+      <c r="W83">
+        <v>1000</v>
+      </c>
+      <c r="X83" t="s">
+        <v>2</v>
+      </c>
+      <c r="Y83">
+        <v>11.086</v>
+      </c>
+      <c r="Z83" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="84" spans="3:26" x14ac:dyDescent="0.25">
       <c r="C84" t="s">
         <v>0</v>
       </c>
@@ -3868,8 +5654,23 @@
       <c r="J84">
         <v>5.5000000000000003E-4</v>
       </c>
-    </row>
-    <row r="85" spans="3:10" x14ac:dyDescent="0.25">
+      <c r="V84" t="s">
+        <v>0</v>
+      </c>
+      <c r="W84">
+        <v>1000</v>
+      </c>
+      <c r="X84" t="s">
+        <v>2</v>
+      </c>
+      <c r="Y84">
+        <v>10.736000000000001</v>
+      </c>
+      <c r="Z84" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="85" spans="3:26" x14ac:dyDescent="0.25">
       <c r="C85" t="s">
         <v>0</v>
       </c>
@@ -3894,8 +5695,23 @@
       <c r="J85">
         <v>5.5000000000000003E-4</v>
       </c>
-    </row>
-    <row r="86" spans="3:10" x14ac:dyDescent="0.25">
+      <c r="V85" t="s">
+        <v>0</v>
+      </c>
+      <c r="W85">
+        <v>1000</v>
+      </c>
+      <c r="X85" t="s">
+        <v>2</v>
+      </c>
+      <c r="Y85">
+        <v>11.016</v>
+      </c>
+      <c r="Z85" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="86" spans="3:26" x14ac:dyDescent="0.25">
       <c r="C86" t="s">
         <v>0</v>
       </c>
@@ -3920,8 +5736,23 @@
       <c r="J86">
         <v>8.3000000000000001E-4</v>
       </c>
-    </row>
-    <row r="87" spans="3:10" x14ac:dyDescent="0.25">
+      <c r="V86" t="s">
+        <v>0</v>
+      </c>
+      <c r="W86">
+        <v>1000</v>
+      </c>
+      <c r="X86" t="s">
+        <v>2</v>
+      </c>
+      <c r="Y86">
+        <v>11.057</v>
+      </c>
+      <c r="Z86" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="87" spans="3:26" x14ac:dyDescent="0.25">
       <c r="C87" t="s">
         <v>0</v>
       </c>
@@ -3946,8 +5777,23 @@
       <c r="J87">
         <v>1.0200000000000001E-3</v>
       </c>
-    </row>
-    <row r="88" spans="3:10" x14ac:dyDescent="0.25">
+      <c r="V87" t="s">
+        <v>0</v>
+      </c>
+      <c r="W87">
+        <v>1000</v>
+      </c>
+      <c r="X87" t="s">
+        <v>2</v>
+      </c>
+      <c r="Y87">
+        <v>10.672000000000001</v>
+      </c>
+      <c r="Z87" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="88" spans="3:26" x14ac:dyDescent="0.25">
       <c r="C88" t="s">
         <v>0</v>
       </c>
@@ -3972,8 +5818,23 @@
       <c r="J88">
         <v>5.5000000000000003E-4</v>
       </c>
-    </row>
-    <row r="89" spans="3:10" x14ac:dyDescent="0.25">
+      <c r="V88" t="s">
+        <v>0</v>
+      </c>
+      <c r="W88">
+        <v>1000</v>
+      </c>
+      <c r="X88" t="s">
+        <v>2</v>
+      </c>
+      <c r="Y88">
+        <v>10.542999999999999</v>
+      </c>
+      <c r="Z88" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="89" spans="3:26" x14ac:dyDescent="0.25">
       <c r="C89" t="s">
         <v>0</v>
       </c>
@@ -3998,8 +5859,23 @@
       <c r="J89">
         <v>5.5000000000000003E-4</v>
       </c>
-    </row>
-    <row r="90" spans="3:10" x14ac:dyDescent="0.25">
+      <c r="V89" t="s">
+        <v>0</v>
+      </c>
+      <c r="W89">
+        <v>1000</v>
+      </c>
+      <c r="X89" t="s">
+        <v>2</v>
+      </c>
+      <c r="Y89">
+        <v>10.826000000000001</v>
+      </c>
+      <c r="Z89" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="90" spans="3:26" x14ac:dyDescent="0.25">
       <c r="C90" t="s">
         <v>0</v>
       </c>
@@ -4024,8 +5900,23 @@
       <c r="J90">
         <v>5.5000000000000003E-4</v>
       </c>
-    </row>
-    <row r="91" spans="3:10" x14ac:dyDescent="0.25">
+      <c r="V90" t="s">
+        <v>0</v>
+      </c>
+      <c r="W90">
+        <v>1000</v>
+      </c>
+      <c r="X90" t="s">
+        <v>2</v>
+      </c>
+      <c r="Y90">
+        <v>11.109</v>
+      </c>
+      <c r="Z90" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="91" spans="3:26" x14ac:dyDescent="0.25">
       <c r="C91" t="s">
         <v>0</v>
       </c>
@@ -4050,8 +5941,23 @@
       <c r="J91">
         <v>5.5000000000000003E-4</v>
       </c>
-    </row>
-    <row r="92" spans="3:10" x14ac:dyDescent="0.25">
+      <c r="V91" t="s">
+        <v>0</v>
+      </c>
+      <c r="W91">
+        <v>1000</v>
+      </c>
+      <c r="X91" t="s">
+        <v>2</v>
+      </c>
+      <c r="Y91">
+        <v>10.984999999999999</v>
+      </c>
+      <c r="Z91" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="92" spans="3:26" x14ac:dyDescent="0.25">
       <c r="C92" t="s">
         <v>0</v>
       </c>
@@ -4076,8 +5982,23 @@
       <c r="J92">
         <v>5.5000000000000003E-4</v>
       </c>
-    </row>
-    <row r="93" spans="3:10" x14ac:dyDescent="0.25">
+      <c r="V92" t="s">
+        <v>0</v>
+      </c>
+      <c r="W92">
+        <v>1000</v>
+      </c>
+      <c r="X92" t="s">
+        <v>2</v>
+      </c>
+      <c r="Y92">
+        <v>11.704000000000001</v>
+      </c>
+      <c r="Z92" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="93" spans="3:26" x14ac:dyDescent="0.25">
       <c r="C93" t="s">
         <v>0</v>
       </c>
@@ -4102,8 +6023,23 @@
       <c r="J93">
         <v>5.5000000000000003E-4</v>
       </c>
-    </row>
-    <row r="94" spans="3:10" x14ac:dyDescent="0.25">
+      <c r="V93" t="s">
+        <v>0</v>
+      </c>
+      <c r="W93">
+        <v>1000</v>
+      </c>
+      <c r="X93" t="s">
+        <v>2</v>
+      </c>
+      <c r="Y93">
+        <v>12.38</v>
+      </c>
+      <c r="Z93" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="94" spans="3:26" x14ac:dyDescent="0.25">
       <c r="C94" t="s">
         <v>0</v>
       </c>
@@ -4128,8 +6064,23 @@
       <c r="J94">
         <v>5.5000000000000003E-4</v>
       </c>
-    </row>
-    <row r="95" spans="3:10" x14ac:dyDescent="0.25">
+      <c r="V94" t="s">
+        <v>0</v>
+      </c>
+      <c r="W94">
+        <v>1000</v>
+      </c>
+      <c r="X94" t="s">
+        <v>2</v>
+      </c>
+      <c r="Y94">
+        <v>11.928000000000001</v>
+      </c>
+      <c r="Z94" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="95" spans="3:26" x14ac:dyDescent="0.25">
       <c r="C95" t="s">
         <v>0</v>
       </c>
@@ -4155,7 +6106,7 @@
         <v>6.0000000000000002E-5</v>
       </c>
     </row>
-    <row r="96" spans="3:10" x14ac:dyDescent="0.25">
+    <row r="96" spans="3:26" x14ac:dyDescent="0.25">
       <c r="C96" t="s">
         <v>0</v>
       </c>
@@ -8810,13 +10761,6 @@
       </c>
     </row>
   </sheetData>
-  <mergeCells count="5">
-    <mergeCell ref="L6:L8"/>
-    <mergeCell ref="N3:S3"/>
-    <mergeCell ref="R4:S4"/>
-    <mergeCell ref="P4:Q4"/>
-    <mergeCell ref="N4:O4"/>
-  </mergeCells>
   <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
   <drawing r:id="rId2"/>

</xml_diff>